<commit_message>
Jisha's changes and some of my own
</commit_message>
<xml_diff>
--- a/experiment_results/all_mcnemar.xlsx
+++ b/experiment_results/all_mcnemar.xlsx
@@ -10,7 +10,7 @@
     <sheet name="mcnemar results" sheetId="2" r:id="rId1"/>
     <sheet name="all_mcnemar" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -684,6 +684,35 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1"/>
+      </a:solidFill>
+      <a:prstDash val="solid"/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:solidFill>
+            <a:schemeClr val="dk1"/>
+          </a:solidFill>
+          <a:latin typeface="+mn-lt"/>
+          <a:ea typeface="+mn-ea"/>
+          <a:cs typeface="+mn-cs"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
 </c:chartSpace>
 </file>
 
@@ -691,7 +720,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="126" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="131" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -702,7 +731,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8678333" cy="6297083"/>
+    <xdr:ext cx="8659752" cy="6289408"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>

</xml_diff>